<commit_message>
Segunda versao da tabela SFS - Kaue
Fiz a descrição do que tinhamos combinado.
</commit_message>
<xml_diff>
--- a/Arquivos Excel/Safe & Sound.xlsx
+++ b/Arquivos Excel/Safe & Sound.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_AulasFiap\Database Modeling and SQL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9750F42D-0D61-472A-B4F8-66814043EF4D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FE488CF9-8989-4629-9DD0-B623EEB20030}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto Safe &amp; Sound" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="80">
   <si>
     <t>NOME DO PROJETO:</t>
   </si>
@@ -350,11 +344,30 @@
   <si>
     <t xml:space="preserve">Número de telefone é uma sequência de números decimais que identificam um ponto de terminação de rede. O número contém as informações necessárias para identificar o ponto final de uma chamada, seja telefônica ou outra. </t>
   </si>
+  <si>
+    <t xml:space="preserve">Número de registro é um número de identificação único e sequencial por funcionário. </t>
+  </si>
+  <si>
+    <t>É o número que identifica qual é conselho que vai registrar, fiscalizar e disciplinar as profissões regulamentadas.</t>
+  </si>
+  <si>
+    <t>Conselho de profissões regulamentadas são conselhos formados por profissionais de cada profissão, com diretorias democraticamente eleitas pelos seus associados que representam os interesses de sua profissão. A sigla vai identificar qual é o conselho.
+Exemplo: CRF, COREN, COFFITO, CRO, CRN, etc.</t>
+  </si>
+  <si>
+    <t>É o status do profissional que vai determinar se o mesmo tem ou não o manejo para o covid-19.</t>
+  </si>
+  <si>
+    <t>Vai descrever se o funcionário está adepto para lidar com o covid-19, se tem os preparos necessários para exercer a função delimitada.</t>
+  </si>
+  <si>
+    <t>É o status do profissional no hospital que vai determinar se o mesmo está ativo ou inativo.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -894,6 +907,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
@@ -903,117 +994,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -1323,35 +1329,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F46E1A1F-27C3-4F3C-A75F-4C8F20A81CA6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.21875" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="48.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
-    <col min="8" max="8" width="30.21875" customWidth="1"/>
-    <col min="18" max="18" width="7.77734375" customWidth="1"/>
-    <col min="19" max="19" width="7.88671875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="48.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" customWidth="1"/>
+    <col min="19" max="19" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -1359,18 +1365,18 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:20" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="53"/>
       <c r="I2" s="7"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -1384,18 +1390,18 @@
       <c r="S2" s="6"/>
       <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="59"/>
       <c r="I3" s="16"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1408,16 +1414,16 @@
       <c r="R3" s="8"/>
       <c r="S3" s="15"/>
     </row>
-    <row r="4" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:20" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="30"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="7"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -1430,7 +1436,7 @@
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:20" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -1440,226 +1446,226 @@
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
     </row>
-    <row r="6" spans="2:20" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="40" t="s">
+    <row r="6" spans="2:20" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="45" t="s">
+      <c r="H6" s="30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:20" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="37" t="s">
+    <row r="7" spans="2:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="G7" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="47" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B8" s="38"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="48" t="s">
+      <c r="F7" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="63"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="49" t="s">
+      <c r="F8" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="2:20" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="38"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="48" t="s">
+      <c r="H8" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="63"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="49" t="s">
+      <c r="E9" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="F9" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="49" t="s">
+      <c r="F9" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="2:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="B10" s="38"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="48" t="s">
+      <c r="H9" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" s="63"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="49" t="s">
+      <c r="E10" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="38"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="48" t="s">
+      <c r="F10" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20" ht="120" x14ac:dyDescent="0.25">
+      <c r="B11" s="63"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="49" t="s">
+      <c r="E11" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="49" t="s">
+      <c r="F11" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="38"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="48" t="s">
+      <c r="H11" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="63"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="F12" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" s="50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="B13" s="38"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="48" t="s">
+      <c r="F12" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20" ht="90" x14ac:dyDescent="0.25">
+      <c r="B13" s="63"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E13" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="49" t="s">
+      <c r="F13" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="2:20" ht="72" x14ac:dyDescent="0.3">
-      <c r="B14" s="38"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="48" t="s">
+      <c r="H13" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20" ht="75" x14ac:dyDescent="0.25">
+      <c r="B14" s="63"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E14" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="49" t="s">
+      <c r="F14" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="H14" s="50" t="s">
+      <c r="H14" s="35" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B15" s="38"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="48" t="s">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="63"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="B16" s="38"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="51" t="s">
+      <c r="E15" s="34"/>
+      <c r="F15" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="63"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="53" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="39"/>
-      <c r="C17" s="36"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="64"/>
+      <c r="C17" s="66"/>
       <c r="D17" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="61"/>
+      <c r="E17" s="45"/>
       <c r="F17" s="14" t="s">
         <v>59</v>
       </c>
@@ -1670,17 +1676,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="37" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="56" t="s">
+      <c r="D18" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="62"/>
+      <c r="E18" s="46"/>
       <c r="F18" s="10" t="s">
         <v>59</v>
       </c>
@@ -1691,13 +1697,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="38"/>
-      <c r="C19" s="35"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="63"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E19" s="63"/>
+      <c r="E19" s="47"/>
       <c r="F19" s="12" t="s">
         <v>59</v>
       </c>
@@ -1708,13 +1714,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="38"/>
-      <c r="C20" s="35"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="63"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="63"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="12" t="s">
         <v>59</v>
       </c>
@@ -1725,13 +1731,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="38"/>
-      <c r="C21" s="35"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="63"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="63"/>
+      <c r="E21" s="47"/>
       <c r="F21" s="12" t="s">
         <v>59</v>
       </c>
@@ -1742,13 +1748,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="38"/>
-      <c r="C22" s="35"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="63"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="63"/>
+      <c r="E22" s="47"/>
       <c r="F22" s="12" t="s">
         <v>59</v>
       </c>
@@ -1759,13 +1765,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="39"/>
-      <c r="C23" s="36"/>
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="64"/>
+      <c r="C23" s="66"/>
       <c r="D23" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E23" s="64"/>
+      <c r="E23" s="48"/>
       <c r="F23" s="19" t="s">
         <v>59</v>
       </c>
@@ -1776,36 +1782,40 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="54" t="s">
+      <c r="B24" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="57" t="s">
+      <c r="D24" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="65"/>
+      <c r="E24" s="49" t="s">
+        <v>74</v>
+      </c>
       <c r="F24" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="59" t="s">
+      <c r="B25" s="60"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="65"/>
+      <c r="E25" s="49" t="s">
+        <v>75</v>
+      </c>
       <c r="F25" s="13" t="s">
         <v>59</v>
       </c>
@@ -1816,68 +1826,76 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="35"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="63"/>
+      <c r="E26" s="47" t="s">
+        <v>76</v>
+      </c>
       <c r="F26" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H26" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="35"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="63"/>
+      <c r="E27" s="47" t="s">
+        <v>78</v>
+      </c>
       <c r="F27" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H27" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H27" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="35"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="63"/>
+      <c r="E28" s="47" t="s">
+        <v>77</v>
+      </c>
       <c r="F28" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G28" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="35"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="66"/>
+      <c r="E29" s="50" t="s">
+        <v>79</v>
+      </c>
       <c r="F29" s="11" t="s">
         <v>59</v>
       </c>
@@ -1889,216 +1907,216 @@
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="D30" s="56" t="s">
+      <c r="D30" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="62"/>
+      <c r="E30" s="46"/>
       <c r="F30" s="10" t="s">
         <v>59</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H30" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="35"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="65"/>
+      <c r="E31" s="49"/>
       <c r="F31" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H31" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H31" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="35"/>
+      <c r="B32" s="63"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="65"/>
+      <c r="E32" s="49"/>
       <c r="F32" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G32" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H32" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H32" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="35"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="61"/>
       <c r="D33" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="65"/>
+      <c r="E33" s="49"/>
       <c r="F33" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H33" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H33" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="35"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="61"/>
       <c r="D34" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="65"/>
+      <c r="E34" s="49"/>
       <c r="F34" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H34" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H34" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="38"/>
-      <c r="C35" s="35"/>
+      <c r="B35" s="63"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="65"/>
+      <c r="E35" s="49"/>
       <c r="F35" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H35" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H35" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="38"/>
-      <c r="C36" s="35"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="65"/>
+      <c r="E36" s="49"/>
       <c r="F36" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H36" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H36" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="38"/>
-      <c r="C37" s="35"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="61"/>
       <c r="D37" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="65"/>
+      <c r="E37" s="49"/>
       <c r="F37" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H37" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H37" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="35"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="61"/>
       <c r="D38" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="49"/>
       <c r="F38" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H38" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H38" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="38"/>
-      <c r="C39" s="35"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="61"/>
       <c r="D39" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E39" s="65"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="13" t="s">
         <v>59</v>
       </c>
       <c r="G39" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H39" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="38"/>
-      <c r="C40" s="35"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="61"/>
       <c r="D40" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="65"/>
+      <c r="E40" s="49"/>
       <c r="F40" s="13" t="s">
         <v>60</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H40" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H40" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22"/>
-      <c r="B41" s="39"/>
-      <c r="C41" s="36"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="66"/>
       <c r="D41" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E41" s="64"/>
+      <c r="E41" s="48"/>
       <c r="F41" s="19" t="s">
         <v>60</v>
       </c>
@@ -2109,208 +2127,208 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="34" t="s">
+      <c r="C42" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="56" t="s">
+      <c r="D42" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="62"/>
+      <c r="E42" s="46"/>
       <c r="F42" s="10" t="s">
         <v>59</v>
       </c>
       <c r="G42" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H42" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H42" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="35"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="61"/>
       <c r="D43" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="63"/>
+      <c r="E43" s="47"/>
       <c r="F43" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H43" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H43" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="35"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="61"/>
       <c r="D44" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E44" s="63"/>
+      <c r="E44" s="47"/>
       <c r="F44" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H44" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H44" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="35"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="61"/>
       <c r="D45" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="63"/>
+      <c r="E45" s="47"/>
       <c r="F45" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H45" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H45" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="35"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="61"/>
       <c r="D46" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E46" s="63"/>
+      <c r="E46" s="47"/>
       <c r="F46" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G46" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H46" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H46" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="35"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="61"/>
       <c r="D47" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="63"/>
+      <c r="E47" s="47"/>
       <c r="F47" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G47" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H47" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H47" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="35"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="61"/>
       <c r="D48" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E48" s="63"/>
+      <c r="E48" s="47"/>
       <c r="F48" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G48" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="H48" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H48" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="22"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="35"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="61"/>
       <c r="D49" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="63"/>
+      <c r="E49" s="47"/>
       <c r="F49" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G49" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H49" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H49" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="35"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="61"/>
       <c r="D50" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="63"/>
+      <c r="E50" s="47"/>
       <c r="F50" s="12" t="s">
         <v>59</v>
       </c>
       <c r="G50" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="H50" s="58" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H50" s="42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22"/>
-      <c r="B51" s="39"/>
-      <c r="C51" s="36"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="66"/>
       <c r="D51" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="E51" s="64"/>
+      <c r="E51" s="48"/>
       <c r="F51" s="19" t="s">
         <v>60</v>
       </c>
       <c r="G51" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="H51" s="58" t="s">
+      <c r="H51" s="42" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="C24:C29"/>
+    <mergeCell ref="B42:B51"/>
+    <mergeCell ref="C42:C51"/>
     <mergeCell ref="B30:B41"/>
     <mergeCell ref="C30:C41"/>
     <mergeCell ref="C7:C17"/>
     <mergeCell ref="B7:B17"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="C18:C23"/>
-    <mergeCell ref="B42:B51"/>
-    <mergeCell ref="C42:C51"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="C24:C29"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:H51">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Terceira versão tabela SFS - Gustavo
Complementação da linha prontuario medico.
</commit_message>
<xml_diff>
--- a/Arquivos Excel/Safe & Sound.xlsx
+++ b/Arquivos Excel/Safe & Sound.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\OneDrive\Área de Trabalho\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C82F7B4-2FEE-417C-BFD8-D121D4B3CE07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto Safe &amp; Sound" sheetId="1" r:id="rId1"/>
@@ -14,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="88">
   <si>
     <t>NOME DO PROJETO:</t>
   </si>
@@ -363,12 +363,37 @@
   <si>
     <t>É o status do profissional no hospital que vai determinar se o mesmo está ativo ou inativo.</t>
   </si>
+  <si>
+    <t>Informação utilizada para indicar a data que o medico ira entrar em contato com o paciente para prosseguir com o tratamento. Formato dd/mm/aaaa. Horario: --:--</t>
+  </si>
+  <si>
+    <t>Informação utilizada para indicar a data que o paciente recebera visitas externas. Formato dd/mm/aaaa. Horario: --:--</t>
+  </si>
+  <si>
+    <t>Nome do paciente, é um antropônimo dado a uma criança ao nascer, no batismo ou em outra ocasião especial.
+Exemplo: Rita de Cássia Rodrigues.</t>
+  </si>
+  <si>
+    <t>É o numero referente ao Cremesp (Conselho Regional de Medicina do Estado de São Paulo) é a entidade responsável por fiscalizar, apurar e julgar irregularidades contra médicos no Estado.</t>
+  </si>
+  <si>
+    <t>É o nome do profissional da saúde autorizado pelo Estado para exercer a Medicina.</t>
+  </si>
+  <si>
+    <t>A anamnese médica é um procedimento fundamental para estabelecer o diagnóstico preciso e instituir as condutas terapêuticas mais adequadas às condições clínicas do paciente.</t>
+  </si>
+  <si>
+    <t>A evolução precisa constar no prontuário a cada visita por todos os profissionais de saúde, sendo um descritivo das ações tomadas e da situação observada do paciente. Obrigatório.</t>
+  </si>
+  <si>
+    <t>A hipótese diagnóstica também não necessita ser preenchida todos os dias. Ela pode mudar conforme evolução do paciente, surgimento de novos sintomas, resultados de exames, etc.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,8 +428,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -429,6 +468,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="34">
     <border>
@@ -763,15 +808,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -845,13 +881,26 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -898,7 +947,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
@@ -964,7 +1013,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -985,34 +1034,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1329,18 +1390,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +1409,7 @@
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.28515625" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.42578125" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
@@ -1369,14 +1430,14 @@
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="7"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -1394,14 +1455,14 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="59"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="65"/>
       <c r="I3" s="16"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1418,12 +1479,12 @@
       <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="56"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="62"/>
       <c r="I4" s="7"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
@@ -1436,7 +1497,7 @@
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="2:20" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -1470,10 +1531,10 @@
       </c>
     </row>
     <row r="7" spans="2:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="54" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="39" t="s">
@@ -1493,8 +1554,8 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="63"/>
-      <c r="C8" s="61"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="55"/>
       <c r="D8" s="33" t="s">
         <v>24</v>
       </c>
@@ -1512,8 +1573,8 @@
       </c>
     </row>
     <row r="9" spans="2:20" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="63"/>
-      <c r="C9" s="61"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="55"/>
       <c r="D9" s="33" t="s">
         <v>25</v>
       </c>
@@ -1531,8 +1592,8 @@
       </c>
     </row>
     <row r="10" spans="2:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="B10" s="63"/>
-      <c r="C10" s="61"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="55"/>
       <c r="D10" s="33" t="s">
         <v>27</v>
       </c>
@@ -1550,8 +1611,8 @@
       </c>
     </row>
     <row r="11" spans="2:20" ht="120" x14ac:dyDescent="0.25">
-      <c r="B11" s="63"/>
-      <c r="C11" s="61"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="55"/>
       <c r="D11" s="33" t="s">
         <v>26</v>
       </c>
@@ -1568,9 +1629,9 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="63"/>
-      <c r="C12" s="61"/>
+    <row r="12" spans="2:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="52"/>
+      <c r="C12" s="55"/>
       <c r="D12" s="33" t="s">
         <v>28</v>
       </c>
@@ -1588,8 +1649,8 @@
       </c>
     </row>
     <row r="13" spans="2:20" ht="90" x14ac:dyDescent="0.25">
-      <c r="B13" s="63"/>
-      <c r="C13" s="61"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="33" t="s">
         <v>29</v>
       </c>
@@ -1607,8 +1668,8 @@
       </c>
     </row>
     <row r="14" spans="2:20" ht="75" x14ac:dyDescent="0.25">
-      <c r="B14" s="63"/>
-      <c r="C14" s="61"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="55"/>
       <c r="D14" s="33" t="s">
         <v>30</v>
       </c>
@@ -1626,8 +1687,8 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B15" s="63"/>
-      <c r="C15" s="61"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="33" t="s">
         <v>31</v>
       </c>
@@ -1643,8 +1704,8 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="63"/>
-      <c r="C16" s="61"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="55"/>
       <c r="D16" s="36" t="s">
         <v>61</v>
       </c>
@@ -1660,8 +1721,8 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="64"/>
-      <c r="C17" s="66"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="56"/>
       <c r="D17" s="14" t="s">
         <v>32</v>
       </c>
@@ -1677,10 +1738,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="62" t="s">
+      <c r="B18" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="C18" s="54" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="40" t="s">
@@ -1698,8 +1759,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="63"/>
-      <c r="C19" s="61"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="12" t="s">
         <v>34</v>
       </c>
@@ -1715,8 +1776,8 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="63"/>
-      <c r="C20" s="61"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="55"/>
       <c r="D20" s="12" t="s">
         <v>35</v>
       </c>
@@ -1732,8 +1793,8 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="63"/>
-      <c r="C21" s="61"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="55"/>
       <c r="D21" s="12" t="s">
         <v>36</v>
       </c>
@@ -1749,8 +1810,8 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="63"/>
-      <c r="C22" s="61"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="55"/>
       <c r="D22" s="12" t="s">
         <v>38</v>
       </c>
@@ -1766,8 +1827,8 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="64"/>
-      <c r="C23" s="66"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="56"/>
       <c r="D23" s="19" t="s">
         <v>39</v>
       </c>
@@ -1784,10 +1845,10 @@
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="61" t="s">
+      <c r="C24" s="55" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="41" t="s">
@@ -1808,8 +1869,8 @@
     </row>
     <row r="25" spans="1:9" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="61"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="55"/>
       <c r="D25" s="43" t="s">
         <v>40</v>
       </c>
@@ -1828,8 +1889,8 @@
     </row>
     <row r="26" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A26" s="22"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="61"/>
+      <c r="B26" s="52"/>
+      <c r="C26" s="55"/>
       <c r="D26" s="12" t="s">
         <v>42</v>
       </c>
@@ -1848,8 +1909,8 @@
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="22"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="61"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="55"/>
       <c r="D27" s="12" t="s">
         <v>43</v>
       </c>
@@ -1868,8 +1929,8 @@
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="61"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="55"/>
       <c r="D28" s="12" t="s">
         <v>37</v>
       </c>
@@ -1888,8 +1949,8 @@
     </row>
     <row r="29" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="61"/>
+      <c r="B29" s="52"/>
+      <c r="C29" s="55"/>
       <c r="D29" s="11" t="s">
         <v>58</v>
       </c>
@@ -1907,18 +1968,20 @@
       </c>
       <c r="I29" s="9"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="22"/>
-      <c r="B30" s="62" t="s">
+      <c r="B30" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="65" t="s">
+      <c r="C30" s="54" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E30" s="46"/>
+      <c r="E30" s="31" t="s">
+        <v>66</v>
+      </c>
       <c r="F30" s="10" t="s">
         <v>59</v>
       </c>
@@ -1929,14 +1992,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="22"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="61"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="55"/>
       <c r="D31" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="49"/>
+      <c r="E31" s="34" t="s">
+        <v>80</v>
+      </c>
       <c r="F31" s="13" t="s">
         <v>59</v>
       </c>
@@ -1947,14 +2012,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="22"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="61"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="55"/>
       <c r="D32" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="49"/>
+      <c r="E32" s="49" t="s">
+        <v>81</v>
+      </c>
       <c r="F32" s="13" t="s">
         <v>59</v>
       </c>
@@ -1965,14 +2032,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="61"/>
+      <c r="B33" s="52"/>
+      <c r="C33" s="55"/>
       <c r="D33" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="49"/>
+      <c r="E33" s="34" t="s">
+        <v>82</v>
+      </c>
       <c r="F33" s="13" t="s">
         <v>59</v>
       </c>
@@ -1983,14 +2052,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A34" s="22"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="61"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="55"/>
       <c r="D34" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="49"/>
+      <c r="E34" s="34" t="s">
+        <v>68</v>
+      </c>
       <c r="F34" s="13" t="s">
         <v>59</v>
       </c>
@@ -2001,14 +2072,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="22"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="61"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="55"/>
       <c r="D35" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="49"/>
+      <c r="E35" s="34" t="s">
+        <v>70</v>
+      </c>
       <c r="F35" s="13" t="s">
         <v>59</v>
       </c>
@@ -2021,12 +2094,14 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="22"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="61"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="55"/>
       <c r="D36" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E36" s="49"/>
+      <c r="E36" s="33" t="s">
+        <v>67</v>
+      </c>
       <c r="F36" s="13" t="s">
         <v>59</v>
       </c>
@@ -2037,14 +2112,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="22"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="61"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="55"/>
       <c r="D37" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="49"/>
+      <c r="E37" s="67" t="s">
+        <v>83</v>
+      </c>
       <c r="F37" s="13" t="s">
         <v>59</v>
       </c>
@@ -2055,14 +2132,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="22"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="61"/>
+      <c r="B38" s="52"/>
+      <c r="C38" s="55"/>
       <c r="D38" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E38" s="49"/>
+      <c r="E38" s="49" t="s">
+        <v>84</v>
+      </c>
       <c r="F38" s="13" t="s">
         <v>59</v>
       </c>
@@ -2073,14 +2152,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
-      <c r="B39" s="63"/>
-      <c r="C39" s="61"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="55"/>
       <c r="D39" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="68" t="s">
+        <v>85</v>
+      </c>
       <c r="F39" s="13" t="s">
         <v>59</v>
       </c>
@@ -2091,14 +2172,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="22"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="61"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="55"/>
       <c r="D40" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="49"/>
+      <c r="E40" s="69" t="s">
+        <v>86</v>
+      </c>
       <c r="F40" s="13" t="s">
         <v>60</v>
       </c>
@@ -2109,14 +2192,16 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="66"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="56"/>
       <c r="D41" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="E41" s="48"/>
+      <c r="E41" s="70" t="s">
+        <v>87</v>
+      </c>
       <c r="F41" s="19" t="s">
         <v>60</v>
       </c>
@@ -2129,16 +2214,16 @@
     </row>
     <row r="42" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22"/>
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="65" t="s">
+      <c r="C42" s="54" t="s">
         <v>19</v>
       </c>
       <c r="D42" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="E42" s="46"/>
+      <c r="E42" s="49"/>
       <c r="F42" s="10" t="s">
         <v>59</v>
       </c>
@@ -2151,8 +2236,8 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="22"/>
-      <c r="B43" s="63"/>
-      <c r="C43" s="61"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="55"/>
       <c r="D43" s="12" t="s">
         <v>56</v>
       </c>
@@ -2169,8 +2254,8 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="22"/>
-      <c r="B44" s="63"/>
-      <c r="C44" s="61"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="55"/>
       <c r="D44" s="12" t="s">
         <v>22</v>
       </c>
@@ -2187,8 +2272,8 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="22"/>
-      <c r="B45" s="63"/>
-      <c r="C45" s="61"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="55"/>
       <c r="D45" s="12" t="s">
         <v>27</v>
       </c>
@@ -2205,8 +2290,8 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="22"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="61"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="55"/>
       <c r="D46" s="12" t="s">
         <v>26</v>
       </c>
@@ -2223,8 +2308,8 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
-      <c r="B47" s="63"/>
-      <c r="C47" s="61"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="55"/>
       <c r="D47" s="12" t="s">
         <v>25</v>
       </c>
@@ -2241,8 +2326,8 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="22"/>
-      <c r="B48" s="63"/>
-      <c r="C48" s="61"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="55"/>
       <c r="D48" s="12" t="s">
         <v>24</v>
       </c>
@@ -2259,8 +2344,8 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="22"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="61"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="55"/>
       <c r="D49" s="12" t="s">
         <v>40</v>
       </c>
@@ -2277,8 +2362,8 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="22"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="61"/>
+      <c r="B50" s="52"/>
+      <c r="C50" s="55"/>
       <c r="D50" s="12" t="s">
         <v>57</v>
       </c>
@@ -2295,8 +2380,8 @@
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="22"/>
-      <c r="B51" s="64"/>
-      <c r="C51" s="66"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="56"/>
       <c r="D51" s="19" t="s">
         <v>50</v>
       </c>
@@ -2307,12 +2392,17 @@
       <c r="G51" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="H51" s="42" t="s">
+      <c r="H51" s="66" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="B24:B29"/>
+    <mergeCell ref="C24:C29"/>
     <mergeCell ref="B42:B51"/>
     <mergeCell ref="C42:C51"/>
     <mergeCell ref="B30:B41"/>
@@ -2321,13 +2411,8 @@
     <mergeCell ref="B7:B17"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="C18:C23"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="B24:B29"/>
-    <mergeCell ref="C24:C29"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:H51">
+  <conditionalFormatting sqref="D7:H36 D38:H38 D37 F37:H37 D42:H51 D39:D41 F39:H41">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
pequenas mudanças e +info em nm_prof_n_medico
mudança de espessura de uma linha e acrescimo de fecha parenteses no escopo. Acréscimo de tipo de atributo (simples ou composto) e cardinalidades do atributo nm_prof_n_medico
</commit_message>
<xml_diff>
--- a/Arquivos Excel/Safe & Sound.xlsx
+++ b/Arquivos Excel/Safe & Sound.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gih_m\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FF9685-A598-4A15-B164-9ED71F3C89BF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEF4FD4-0D8B-438A-9079-437F3EA58420}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto Safe&amp;Sound" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="82">
   <si>
     <t>NOME DO PROJETO:</t>
   </si>
@@ -457,9 +457,6 @@
     <t>O nome completo do profissional de saúde. Seu conteúdo é sempre obrigatório.</t>
   </si>
   <si>
-    <t>Este produto tem como finalidade permitir o registro em prontuário através de um assistente de voz adaptado à área da saúde que transcreve em texto o que é dito pelo usuário. Também permite a leitura de texto pelo assistente de voz quando solicitada uma informação do prontuário pelo usuário. O produto objetiva diminuir o número de interações do usuário com superfícies (teclados, prontuários físicos, desparamentações, etc. em ambientes com alta carga viral de covid-19, ao mesmo tempo que permite a manutenção do prontuário a beira leito sem necessidade de produzir documentação retroativa.</t>
-  </si>
-  <si>
     <t>• Abrir o cadastro dos pacientes com informações mínimas para identificação segura do paciente;
 • Abrir o cadastro de médicos que podem atuar na instituição;
 • Abrir o cadastro de profissionais de saúde não médicos (enfermeiros, psicólogos, farmacêuticos, fisioterapeutas,etc) do hospital;
@@ -493,6 +490,9 @@
   </si>
   <si>
     <t>O cadastro do número de telefone é necessário para contatar familiares, dependentes ou responsáveis pelo paciente. Podem ser cadastrados mais de um telefone.</t>
+  </si>
+  <si>
+    <t>Este produto tem como finalidade permitir o registro em prontuário através de um assistente de voz adaptado à área da saúde que transcreve em texto o que é dito pelo usuário. Também permite a leitura de texto pelo assistente de voz quando solicitada uma informação do prontuário pelo usuário. O produto objetiva diminuir o número de interações do usuário com superfícies (teclados, prontuários físicos, desparamentações etc.) em ambientes com alta carga viral de covid-19, ao mesmo tempo que permite a manutenção do prontuário a beira leito sem necessidade de produzir documentação retroativa.</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -979,11 +979,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1118,6 +1131,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1127,39 +1146,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1560,37 +1581,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F60B7E-595C-4DED-A8B7-7A6F54C6BC44}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:A13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.1796875" customWidth="1"/>
-    <col min="2" max="2" width="54.1796875" customWidth="1"/>
-    <col min="3" max="3" width="30.36328125" customWidth="1"/>
-    <col min="4" max="4" width="48.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7265625" customWidth="1"/>
-    <col min="7" max="7" width="30.26953125" customWidth="1"/>
-    <col min="8" max="15" width="8.54296875" customWidth="1"/>
-    <col min="16" max="16" width="7.7265625" customWidth="1"/>
-    <col min="17" max="17" width="7.81640625" customWidth="1"/>
-    <col min="18" max="1023" width="8.54296875" customWidth="1"/>
+    <col min="1" max="1" width="44.21875" customWidth="1"/>
+    <col min="2" max="2" width="54.21875" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="48.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="7" max="7" width="30.21875" customWidth="1"/>
+    <col min="8" max="15" width="8.5546875" customWidth="1"/>
+    <col min="16" max="17" width="7.77734375" customWidth="1"/>
+    <col min="18" max="1023" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1603,18 +1623,18 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="57" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
+      <c r="B2" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1626,18 +1646,18 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
+      <c r="B3" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1649,7 +1669,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -1660,7 +1680,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:18" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>47</v>
       </c>
@@ -1683,11 +1703,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="53" t="s">
+    <row r="6" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="57" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -1706,9 +1726,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="70" x14ac:dyDescent="0.35">
-      <c r="A7" s="50"/>
-      <c r="B7" s="51"/>
+    <row r="7" spans="1:18" ht="69" x14ac:dyDescent="0.3">
+      <c r="A7" s="52"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="21" t="s">
         <v>16</v>
       </c>
@@ -1725,9 +1745,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="98" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="B8" s="51"/>
+    <row r="8" spans="1:18" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="52"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="22" t="s">
         <v>19</v>
       </c>
@@ -1744,14 +1764,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="150" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="51"/>
+    <row r="9" spans="1:18" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="52"/>
+      <c r="B9" s="54"/>
       <c r="C9" s="21" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>13</v>
@@ -1763,9 +1783,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="120.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="51"/>
+    <row r="10" spans="1:18" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="52"/>
+      <c r="B10" s="54"/>
       <c r="C10" s="46" t="s">
         <v>59</v>
       </c>
@@ -1782,14 +1802,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="50"/>
-      <c r="B11" s="51"/>
+    <row r="11" spans="1:18" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="52"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E11" s="22" t="s">
         <v>13</v>
@@ -1801,9 +1821,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="50"/>
-      <c r="B12" s="51"/>
+    <row r="12" spans="1:18" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="52"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="21" t="s">
         <v>22</v>
       </c>
@@ -1820,14 +1840,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="54"/>
-      <c r="B13" s="56"/>
+    <row r="13" spans="1:18" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="53"/>
+      <c r="B13" s="55"/>
       <c r="C13" s="21" t="s">
         <v>25</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="22" t="s">
         <v>24</v>
@@ -1839,11 +1859,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="126" x14ac:dyDescent="0.35">
-      <c r="A14" s="53" t="s">
+    <row r="14" spans="1:18" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="57" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="44" t="s">
@@ -1862,9 +1882,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="28" x14ac:dyDescent="0.35">
-      <c r="A15" s="50"/>
-      <c r="B15" s="51"/>
+    <row r="15" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="52"/>
+      <c r="B15" s="54"/>
       <c r="C15" s="29" t="s">
         <v>28</v>
       </c>
@@ -1881,9 +1901,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="56" x14ac:dyDescent="0.35">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51"/>
+    <row r="16" spans="1:18" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="52"/>
+      <c r="B16" s="54"/>
       <c r="C16" s="29" t="s">
         <v>29</v>
       </c>
@@ -1900,9 +1920,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="98.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="54"/>
-      <c r="B17" s="56"/>
+    <row r="17" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="53"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="47" t="s">
         <v>55</v>
       </c>
@@ -1919,17 +1939,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="70" x14ac:dyDescent="0.35">
-      <c r="A18" s="53" t="s">
+    <row r="18" spans="1:7" ht="69" x14ac:dyDescent="0.3">
+      <c r="A18" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="57" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="48" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="27" t="s">
@@ -1938,26 +1958,32 @@
       <c r="F18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="62" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A19" s="50"/>
-      <c r="B19" s="51"/>
+      <c r="G18" s="49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="52"/>
+      <c r="B19" s="54"/>
       <c r="C19" s="29" t="s">
         <v>45</v>
       </c>
       <c r="D19" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="30"/>
-    </row>
-    <row r="20" spans="1:7" ht="42" x14ac:dyDescent="0.35">
-      <c r="A20" s="50"/>
-      <c r="B20" s="51"/>
+      <c r="E19" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="54"/>
       <c r="C20" s="33" t="s">
         <v>31</v>
       </c>
@@ -1974,9 +2000,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="98" x14ac:dyDescent="0.35">
-      <c r="A21" s="50"/>
-      <c r="B21" s="51"/>
+    <row r="21" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
+      <c r="B21" s="54"/>
       <c r="C21" s="29" t="s">
         <v>33</v>
       </c>
@@ -1993,9 +2019,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="98.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="54"/>
-      <c r="B22" s="56"/>
+    <row r="22" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="53"/>
+      <c r="B22" s="55"/>
       <c r="C22" s="47" t="s">
         <v>55</v>
       </c>
@@ -2012,11 +2038,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="50" t="s">
+    <row r="23" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="54" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="31" t="s">
@@ -2035,9 +2061,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="56" x14ac:dyDescent="0.35">
-      <c r="A24" s="50"/>
-      <c r="B24" s="51"/>
+    <row r="24" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="52"/>
+      <c r="B24" s="54"/>
       <c r="C24" s="29" t="s">
         <v>36</v>
       </c>
@@ -2054,9 +2080,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="98" x14ac:dyDescent="0.35">
-      <c r="A25" s="50"/>
-      <c r="B25" s="51"/>
+    <row r="25" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="52"/>
+      <c r="B25" s="54"/>
       <c r="C25" s="22" t="s">
         <v>19</v>
       </c>
@@ -2073,9 +2099,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="112" x14ac:dyDescent="0.35">
-      <c r="A26" s="50"/>
-      <c r="B26" s="51"/>
+    <row r="26" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="52"/>
+      <c r="B26" s="54"/>
       <c r="C26" s="21" t="s">
         <v>58</v>
       </c>
@@ -2092,9 +2118,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="140" x14ac:dyDescent="0.35">
-      <c r="A27" s="50"/>
-      <c r="B27" s="51"/>
+    <row r="27" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+      <c r="A27" s="52"/>
+      <c r="B27" s="54"/>
       <c r="C27" s="21" t="s">
         <v>18</v>
       </c>
@@ -2111,13 +2137,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="50"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="21" t="s">
+    <row r="28" spans="1:7" ht="69" x14ac:dyDescent="0.3">
+      <c r="A28" s="52"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="62" t="s">
         <v>57</v>
       </c>
       <c r="E28" s="32" t="s">
@@ -2130,13 +2156,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="126" x14ac:dyDescent="0.35">
-      <c r="A29" s="50"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="58" t="s">
+    <row r="29" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="52"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="59" t="s">
+      <c r="D29" s="64" t="s">
         <v>61</v>
       </c>
       <c r="E29" s="32" t="s">
@@ -2149,9 +2175,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="28" x14ac:dyDescent="0.35">
-      <c r="A30" s="50"/>
-      <c r="B30" s="51"/>
+    <row r="30" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="52"/>
+      <c r="B30" s="54"/>
       <c r="C30" s="29" t="s">
         <v>28</v>
       </c>
@@ -2168,9 +2194,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="70" x14ac:dyDescent="0.35">
-      <c r="A31" s="50"/>
-      <c r="B31" s="51"/>
+    <row r="31" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="52"/>
+      <c r="B31" s="54"/>
       <c r="C31" s="29" t="s">
         <v>37</v>
       </c>
@@ -2187,9 +2213,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="56" x14ac:dyDescent="0.35">
-      <c r="A32" s="50"/>
-      <c r="B32" s="51"/>
+    <row r="32" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="52"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="29" t="s">
         <v>38</v>
       </c>
@@ -2206,9 +2232,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="98.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="54"/>
-      <c r="B33" s="56"/>
+    <row r="33" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="53"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="24" t="s">
         <v>40</v>
       </c>
@@ -2225,11 +2251,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="48" t="s">
+    <row r="34" spans="1:7" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="49" t="s">
+      <c r="B34" s="51" t="s">
         <v>70</v>
       </c>
       <c r="C34" s="26" t="s">
@@ -2248,9 +2274,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="48"/>
-      <c r="B35" s="49"/>
+    <row r="35" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="50"/>
+      <c r="B35" s="51"/>
       <c r="C35" s="29" t="s">
         <v>72</v>
       </c>
@@ -2267,9 +2293,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="48"/>
-      <c r="B36" s="49"/>
+    <row r="36" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="50"/>
+      <c r="B36" s="51"/>
       <c r="C36" s="29" t="s">
         <v>43</v>
       </c>
@@ -2286,9 +2312,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="48"/>
-      <c r="B37" s="49"/>
+    <row r="37" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="50"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="29" t="s">
         <v>19</v>
       </c>
@@ -2305,9 +2331,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="112.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="48"/>
-      <c r="B38" s="49"/>
+    <row r="38" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="50"/>
+      <c r="B38" s="51"/>
       <c r="C38" s="21" t="s">
         <v>58</v>
       </c>
@@ -2324,9 +2350,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="48"/>
-      <c r="B39" s="49"/>
+    <row r="39" spans="1:7" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="50"/>
+      <c r="B39" s="51"/>
       <c r="C39" s="29" t="s">
         <v>18</v>
       </c>
@@ -2343,9 +2369,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="48"/>
-      <c r="B40" s="49"/>
+    <row r="40" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="50"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="21" t="s">
         <v>16</v>
       </c>
@@ -2362,9 +2388,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="48"/>
-      <c r="B41" s="49"/>
+    <row r="41" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="50"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="29" t="s">
         <v>31</v>
       </c>
@@ -2381,9 +2407,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="40.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="48"/>
-      <c r="B42" s="49"/>
+    <row r="42" spans="1:7" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="50"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="29" t="s">
         <v>45</v>
       </c>
@@ -2400,9 +2426,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="48"/>
-      <c r="B43" s="49"/>
+    <row r="43" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="50"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="24" t="s">
         <v>38</v>
       </c>
@@ -2421,12 +2447,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="B34:B43"/>
-    <mergeCell ref="A23:A33"/>
-    <mergeCell ref="B23:B33"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="B1:G1"/>
@@ -2434,6 +2454,12 @@
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="A6:A13"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="B34:B43"/>
+    <mergeCell ref="A23:A33"/>
+    <mergeCell ref="B23:B33"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
   </mergeCells>
   <conditionalFormatting sqref="E29:G29 C31:C33 E31:G33 C30:G30 C6:G28 C34:G43">
     <cfRule type="expression" dxfId="1" priority="2">

</xml_diff>

<commit_message>
Versão final tabela Safe & Sound
acréscimo de nossos nomes e RMs para que pudesse ser entregue
</commit_message>
<xml_diff>
--- a/Arquivos Excel/Safe & Sound.xlsx
+++ b/Arquivos Excel/Safe & Sound.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gih_m\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEF4FD4-0D8B-438A-9079-437F3EA58420}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4985AA57-120B-4A6D-8FAF-90D60595A731}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto Safe&amp;Sound" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Projeto Safe&amp;Sound'!$A$1:$G$47</definedName>
+  </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="83">
   <si>
     <t>NOME DO PROJETO:</t>
   </si>
@@ -494,6 +497,27 @@
   <si>
     <t>Este produto tem como finalidade permitir o registro em prontuário através de um assistente de voz adaptado à área da saúde que transcreve em texto o que é dito pelo usuário. Também permite a leitura de texto pelo assistente de voz quando solicitada uma informação do prontuário pelo usuário. O produto objetiva diminuir o número de interações do usuário com superfícies (teclados, prontuários físicos, desparamentações etc.) em ambientes com alta carga viral de covid-19, ao mesmo tempo que permite a manutenção do prontuário a beira leito sem necessidade de produzir documentação retroativa.</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Integrantes:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="15"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Daniel Sanchez Melero (85109), Giovanna de Mello Leiva (85817), Gustavo Pereira dos Santos (85937), Kauê Augusto Miranda Santos (85707) e Larissa Alves da Silva (86351)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -502,7 +526,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -547,6 +571,25 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -586,7 +629,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -992,11 +1035,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1113,9 +1178,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1137,50 +1199,68 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1579,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F60B7E-595C-4DED-A8B7-7A6F54C6BC44}">
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1599,18 +1679,18 @@
     <col min="18" max="1023" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1623,18 +1703,18 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1646,18 +1726,18 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="81.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1703,11 +1783,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="56" t="s">
+    <row r="6" spans="1:18" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="56" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -1727,8 +1807,8 @@
       </c>
     </row>
     <row r="7" spans="1:18" ht="69" x14ac:dyDescent="0.3">
-      <c r="A7" s="52"/>
-      <c r="B7" s="54"/>
+      <c r="A7" s="54"/>
+      <c r="B7" s="57"/>
       <c r="C7" s="21" t="s">
         <v>16</v>
       </c>
@@ -1746,8 +1826,8 @@
       </c>
     </row>
     <row r="8" spans="1:18" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="52"/>
-      <c r="B8" s="54"/>
+      <c r="A8" s="54"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="22" t="s">
         <v>19</v>
       </c>
@@ -1764,9 +1844,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="150" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="52"/>
-      <c r="B9" s="54"/>
+    <row r="9" spans="1:18" ht="138" x14ac:dyDescent="0.3">
+      <c r="A9" s="54"/>
+      <c r="B9" s="57"/>
       <c r="C9" s="21" t="s">
         <v>18</v>
       </c>
@@ -1783,10 +1863,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="46" t="s">
+    <row r="10" spans="1:18" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="54"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="45" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="37" t="s">
@@ -1802,9 +1882,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="52"/>
-      <c r="B11" s="54"/>
+    <row r="11" spans="1:18" ht="69" x14ac:dyDescent="0.3">
+      <c r="A11" s="54"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
@@ -1821,9 +1901,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
-      <c r="B12" s="54"/>
+    <row r="12" spans="1:18" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="54"/>
+      <c r="B12" s="57"/>
       <c r="C12" s="21" t="s">
         <v>22</v>
       </c>
@@ -1840,9 +1920,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="53"/>
-      <c r="B13" s="55"/>
+    <row r="13" spans="1:18" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="55"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="21" t="s">
         <v>25</v>
       </c>
@@ -1860,16 +1940,16 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="44" t="s">
+      <c r="C14" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="44" t="s">
         <v>61</v>
       </c>
       <c r="E14" s="27" t="s">
@@ -1883,8 +1963,8 @@
       </c>
     </row>
     <row r="15" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="52"/>
-      <c r="B15" s="54"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="29" t="s">
         <v>28</v>
       </c>
@@ -1902,8 +1982,8 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="52"/>
-      <c r="B16" s="54"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="29" t="s">
         <v>29</v>
       </c>
@@ -1921,9 +2001,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="53"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="47" t="s">
+      <c r="A17" s="55"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="46" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="39" t="s">
@@ -1940,16 +2020,16 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="69" x14ac:dyDescent="0.3">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="56" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="48" t="s">
+      <c r="D18" s="47" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="27" t="s">
@@ -1958,13 +2038,13 @@
       <c r="F18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="49" t="s">
+      <c r="G18" s="48" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="52"/>
-      <c r="B19" s="54"/>
+      <c r="A19" s="54"/>
+      <c r="B19" s="57"/>
       <c r="C19" s="29" t="s">
         <v>45</v>
       </c>
@@ -1982,8 +2062,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="52"/>
-      <c r="B20" s="54"/>
+      <c r="A20" s="54"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="33" t="s">
         <v>31</v>
       </c>
@@ -2001,8 +2081,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="52"/>
-      <c r="B21" s="54"/>
+      <c r="A21" s="54"/>
+      <c r="B21" s="57"/>
       <c r="C21" s="29" t="s">
         <v>33</v>
       </c>
@@ -2020,9 +2100,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="53"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="47" t="s">
+      <c r="A22" s="55"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="46" t="s">
         <v>55</v>
       </c>
       <c r="D22" s="39" t="s">
@@ -2038,11 +2118,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="52" t="s">
+    <row r="23" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="54" t="s">
+      <c r="B23" s="56" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="31" t="s">
@@ -2062,8 +2142,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="52"/>
-      <c r="B24" s="54"/>
+      <c r="A24" s="54"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="29" t="s">
         <v>36</v>
       </c>
@@ -2081,8 +2161,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
-      <c r="B25" s="54"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="22" t="s">
         <v>19</v>
       </c>
@@ -2099,9 +2179,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="52"/>
-      <c r="B26" s="54"/>
+    <row r="26" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="69"/>
+      <c r="B26" s="58"/>
       <c r="C26" s="21" t="s">
         <v>58</v>
       </c>
@@ -2118,265 +2198,273 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="138" x14ac:dyDescent="0.3">
-      <c r="A27" s="52"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="21" t="s">
+    <row r="27" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="138" x14ac:dyDescent="0.3">
+      <c r="A28" s="53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D28" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="32" t="s">
+      <c r="E28" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="69" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="61" t="s">
+      <c r="G28" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="69" x14ac:dyDescent="0.3">
+      <c r="A29" s="54"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="62" t="s">
+      <c r="D29" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="E28" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="32" t="s">
+      <c r="E29" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="63" t="s">
+      <c r="G29" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="54"/>
+      <c r="B30" s="57"/>
+      <c r="C30" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="64" t="s">
+      <c r="D30" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="29" t="s">
+      <c r="E30" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="54"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="38" t="s">
+      <c r="D31" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="52"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="29" t="s">
+      <c r="E31" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="54"/>
+      <c r="B32" s="57"/>
+      <c r="C32" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="41" t="s">
+      <c r="D32" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A32" s="52"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="29" t="s">
+      <c r="E32" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="54"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="42" t="s">
+      <c r="D33" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="E33" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F32" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="53"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="24" t="s">
+      <c r="F33" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="55"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="39" t="s">
+      <c r="D34" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E34" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="F34" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="G33" s="25" t="s">
+      <c r="G34" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="50" t="s">
+    <row r="35" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="B35" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C35" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D35" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="50"/>
-      <c r="B35" s="51"/>
-      <c r="C35" s="29" t="s">
+      <c r="E35" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="62"/>
+      <c r="B36" s="63"/>
+      <c r="C36" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D36" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="50"/>
-      <c r="B36" s="51"/>
-      <c r="C36" s="29" t="s">
+      <c r="E36" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="62"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D37" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="E36" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="50"/>
-      <c r="B37" s="51"/>
-      <c r="C37" s="29" t="s">
+      <c r="E37" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="62"/>
+      <c r="B38" s="63"/>
+      <c r="C38" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D37" s="38" t="s">
+      <c r="D38" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="E37" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="50"/>
-      <c r="B38" s="51"/>
-      <c r="C38" s="21" t="s">
+      <c r="E38" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="62"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="37" t="s">
+      <c r="D39" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="50"/>
-      <c r="B39" s="51"/>
-      <c r="C39" s="29" t="s">
+      <c r="E39" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="62"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D39" s="38" t="s">
+      <c r="D40" s="38" t="s">
         <v>44</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="50"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D40" s="37" t="s">
-        <v>57</v>
       </c>
       <c r="E40" s="29" t="s">
         <v>13</v>
@@ -2388,65 +2476,104 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="50"/>
-      <c r="B41" s="51"/>
-      <c r="C41" s="29" t="s">
+    <row r="41" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="62"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="62"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="43" t="s">
+      <c r="D42" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="E41" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="50"/>
-      <c r="B42" s="51"/>
-      <c r="C42" s="29" t="s">
+      <c r="E42" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="62"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="38" t="s">
+      <c r="D43" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E42" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="50"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="24" t="s">
+      <c r="E43" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="62"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="D44" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="E44" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F43" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="35" t="s">
-        <v>15</v>
-      </c>
+      <c r="F44" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A46" s="67" t="s">
+        <v>82</v>
+      </c>
+      <c r="B46" s="66"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="66"/>
+      <c r="G46" s="66"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A35:A44"/>
+    <mergeCell ref="B35:B44"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B28:B34"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="B1:G1"/>
@@ -2454,24 +2581,21 @@
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="A6:A13"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="B34:B43"/>
-    <mergeCell ref="A23:A33"/>
-    <mergeCell ref="B23:B33"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
   </mergeCells>
-  <conditionalFormatting sqref="E29:G29 C31:C33 E31:G33 C30:G30 C6:G28 C34:G43">
+  <conditionalFormatting sqref="E30:G30 C32:C34 E32:G34 C31:G31 C6:G26 C35:G44 C28:G29">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29:D29">
+  <conditionalFormatting sqref="C30:D30">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="36" orientation="portrait" r:id="rId1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="26" max="16383" man="1"/>
+  </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Versão entregue para a professora
ajustes na tabela e acréscimo dos nomes e rms dos integrantes do grupo
</commit_message>
<xml_diff>
--- a/Arquivos Excel/Safe & Sound.xlsx
+++ b/Arquivos Excel/Safe & Sound.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gih_m\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4985AA57-120B-4A6D-8FAF-90D60595A731}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C531264-672B-4AED-BC2F-8B38C0727A2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto Safe&amp;Sound" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Projeto Safe&amp;Sound'!$A$1:$G$47</definedName>
-  </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="83">
   <si>
     <t>NOME DO PROJETO:</t>
   </si>
@@ -500,22 +497,22 @@
   <si>
     <r>
       <rPr>
-        <sz val="15"/>
+        <sz val="16"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Integrantes:</t>
+      <t xml:space="preserve">Integrantes: </t>
     </r>
     <r>
       <rPr>
-        <sz val="15"/>
+        <sz val="16"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> Daniel Sanchez Melero (85109), Giovanna de Mello Leiva (85817), Gustavo Pereira dos Santos (85937), Kauê Augusto Miranda Santos (85707) e Larissa Alves da Silva (86351)</t>
+      <t>Daniel Sanchez Melero (85109), Giovanna de Mello Leiva (85817), Gustavo Pereira dos Santos (85937), Kauê Augusto Miranda Santos (85707) e Larissa Alves da Silva (86351)</t>
     </r>
   </si>
 </sst>
@@ -526,7 +523,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -572,20 +569,20 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -629,7 +626,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1035,33 +1032,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1178,6 +1153,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1244,23 +1222,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1659,13 +1625,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F60B7E-595C-4DED-A8B7-7A6F54C6BC44}">
-  <dimension ref="A1:R46"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B44"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="44.21875" customWidth="1"/>
     <col min="2" max="2" width="54.21875" customWidth="1"/>
@@ -1679,18 +1645,18 @@
     <col min="18" max="1023" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="20.399999999999999" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1703,18 +1669,18 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="46.95" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1726,18 +1692,18 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="81.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="81.75" customHeight="1" thickBot="1">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1749,7 +1715,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="15" thickBot="1">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -1760,7 +1726,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:18" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="83.4" thickBot="1">
       <c r="A5" s="12" t="s">
         <v>47</v>
       </c>
@@ -1783,11 +1749,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
+    <row r="6" spans="1:18" ht="49.5" customHeight="1">
+      <c r="A6" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="57" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -1806,9 +1772,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="69" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="57"/>
+    <row r="7" spans="1:18" ht="69">
+      <c r="A7" s="55"/>
+      <c r="B7" s="58"/>
       <c r="C7" s="21" t="s">
         <v>16</v>
       </c>
@@ -1825,9 +1791,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="57"/>
+    <row r="8" spans="1:18" ht="96.6">
+      <c r="A8" s="55"/>
+      <c r="B8" s="58"/>
       <c r="C8" s="22" t="s">
         <v>19</v>
       </c>
@@ -1844,9 +1810,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="138" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="57"/>
+    <row r="9" spans="1:18" ht="150" customHeight="1">
+      <c r="A9" s="55"/>
+      <c r="B9" s="58"/>
       <c r="C9" s="21" t="s">
         <v>18</v>
       </c>
@@ -1863,10 +1829,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="45" t="s">
+    <row r="10" spans="1:18" ht="120.75" customHeight="1">
+      <c r="A10" s="55"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="46" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="37" t="s">
@@ -1882,9 +1848,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="69" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
-      <c r="B11" s="57"/>
+    <row r="11" spans="1:18" ht="66.75" customHeight="1">
+      <c r="A11" s="55"/>
+      <c r="B11" s="58"/>
       <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
@@ -1901,9 +1867,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
-      <c r="B12" s="57"/>
+    <row r="12" spans="1:18" ht="90" customHeight="1">
+      <c r="A12" s="55"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="21" t="s">
         <v>22</v>
       </c>
@@ -1920,9 +1886,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="58"/>
+    <row r="13" spans="1:18" ht="79.5" customHeight="1" thickBot="1">
+      <c r="A13" s="56"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="21" t="s">
         <v>25</v>
       </c>
@@ -1939,17 +1905,17 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="53" t="s">
+    <row r="14" spans="1:18" ht="124.2">
+      <c r="A14" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="45" t="s">
         <v>61</v>
       </c>
       <c r="E14" s="27" t="s">
@@ -1962,9 +1928,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="54"/>
-      <c r="B15" s="57"/>
+    <row r="15" spans="1:18" ht="27.6">
+      <c r="A15" s="55"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="29" t="s">
         <v>28</v>
       </c>
@@ -1981,9 +1947,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="54"/>
-      <c r="B16" s="57"/>
+    <row r="16" spans="1:18" ht="55.2">
+      <c r="A16" s="55"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="29" t="s">
         <v>29</v>
       </c>
@@ -2000,10 +1966,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="55"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="46" t="s">
+    <row r="17" spans="1:7" ht="97.2" thickBot="1">
+      <c r="A17" s="56"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="47" t="s">
         <v>55</v>
       </c>
       <c r="D17" s="39" t="s">
@@ -2019,17 +1985,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="69" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+    <row r="18" spans="1:7" ht="69">
+      <c r="A18" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="57" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="47" t="s">
+      <c r="D18" s="48" t="s">
         <v>63</v>
       </c>
       <c r="E18" s="27" t="s">
@@ -2038,13 +2004,13 @@
       <c r="F18" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="48" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
-      <c r="B19" s="57"/>
+      <c r="G18" s="49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="27.6">
+      <c r="A19" s="55"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="29" t="s">
         <v>45</v>
       </c>
@@ -2061,9 +2027,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
-      <c r="B20" s="57"/>
+    <row r="20" spans="1:7" ht="41.4">
+      <c r="A20" s="55"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="33" t="s">
         <v>31</v>
       </c>
@@ -2080,9 +2046,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="57"/>
+    <row r="21" spans="1:7" ht="96.6">
+      <c r="A21" s="55"/>
+      <c r="B21" s="58"/>
       <c r="C21" s="29" t="s">
         <v>33</v>
       </c>
@@ -2099,10 +2065,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="55"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="46" t="s">
+    <row r="22" spans="1:7" ht="97.2" thickBot="1">
+      <c r="A22" s="56"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="47" t="s">
         <v>55</v>
       </c>
       <c r="D22" s="39" t="s">
@@ -2118,11 +2084,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="53" t="s">
+    <row r="23" spans="1:7" ht="45" customHeight="1">
+      <c r="A23" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="58" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="31" t="s">
@@ -2141,9 +2107,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
-      <c r="B24" s="57"/>
+    <row r="24" spans="1:7" ht="55.2">
+      <c r="A24" s="55"/>
+      <c r="B24" s="58"/>
       <c r="C24" s="29" t="s">
         <v>36</v>
       </c>
@@ -2160,9 +2126,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
-      <c r="B25" s="57"/>
+    <row r="25" spans="1:7" ht="96.6">
+      <c r="A25" s="55"/>
+      <c r="B25" s="58"/>
       <c r="C25" s="22" t="s">
         <v>19</v>
       </c>
@@ -2179,8 +2145,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="69"/>
+    <row r="26" spans="1:7" ht="110.4">
+      <c r="A26" s="55"/>
       <c r="B26" s="58"/>
       <c r="C26" s="21" t="s">
         <v>58</v>
@@ -2198,273 +2164,265 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="83.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="68" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="138" x14ac:dyDescent="0.3">
-      <c r="A28" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="56" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="64" t="s">
+    <row r="27" spans="1:7" ht="138">
+      <c r="A27" s="55"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D27" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="27" t="s">
+      <c r="E27" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="28" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="69" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
-      <c r="B29" s="57"/>
-      <c r="C29" s="49" t="s">
+      <c r="G27" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="69">
+      <c r="A28" s="55"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="50" t="s">
+      <c r="D28" s="51" t="s">
         <v>57</v>
       </c>
+      <c r="E28" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="G28" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="124.2">
+      <c r="A29" s="55"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" s="53" t="s">
+        <v>61</v>
+      </c>
       <c r="E29" s="32" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="27.6">
+      <c r="A30" s="55"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="69">
+      <c r="A31" s="55"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="55.2">
+      <c r="A32" s="55"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="97.2" thickBot="1">
+      <c r="A33" s="56"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="G29" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="51" t="s">
-        <v>67</v>
-      </c>
-      <c r="D30" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G30" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="D31" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G31" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
-      <c r="B32" s="57"/>
-      <c r="C32" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="54"/>
-      <c r="B33" s="57"/>
-      <c r="C33" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="97.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="55"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D34" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="24" t="s">
+      <c r="G33" s="25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="41.1" customHeight="1" thickBot="1">
+      <c r="A34" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="G34" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="55.8" thickBot="1">
+      <c r="A35" s="63"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="42" thickBot="1">
+      <c r="A36" s="63"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="69.599999999999994" thickBot="1">
+      <c r="A37" s="63"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="111" thickBot="1">
+      <c r="A38" s="63"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="58.95" customHeight="1" thickBot="1">
+      <c r="A39" s="63"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="G34" s="25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="63" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="62"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="62"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="62"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="D38" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="111" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="62"/>
-      <c r="B39" s="63"/>
-      <c r="C39" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E39" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>14</v>
-      </c>
       <c r="G39" s="34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="62"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="D40" s="38" t="s">
-        <v>44</v>
+    <row r="40" spans="1:7" ht="69.599999999999994" thickBot="1">
+      <c r="A40" s="63"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>57</v>
       </c>
       <c r="E40" s="29" t="s">
         <v>13</v>
@@ -2476,33 +2434,33 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="62"/>
-      <c r="B41" s="63"/>
-      <c r="C41" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="37" t="s">
-        <v>57</v>
+    <row r="41" spans="1:7" ht="42" thickBot="1">
+      <c r="A41" s="63"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="43" t="s">
+        <v>32</v>
       </c>
       <c r="E41" s="29" t="s">
         <v>13</v>
       </c>
       <c r="F41" s="29" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G41" s="34" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="62"/>
-      <c r="B42" s="63"/>
+    <row r="42" spans="1:7" ht="40.200000000000003" customHeight="1" thickBot="1">
+      <c r="A42" s="63"/>
+      <c r="B42" s="64"/>
       <c r="C42" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="42" t="s">
-        <v>32</v>
+        <v>45</v>
+      </c>
+      <c r="D42" s="38" t="s">
+        <v>76</v>
       </c>
       <c r="E42" s="29" t="s">
         <v>13</v>
@@ -2514,66 +2472,45 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="62"/>
-      <c r="B43" s="63"/>
-      <c r="C43" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E43" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F43" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="G43" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="62"/>
-      <c r="B44" s="63"/>
-      <c r="C44" s="24" t="s">
+    <row r="43" spans="1:7" ht="69.599999999999994" thickBot="1">
+      <c r="A43" s="63"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="39" t="s">
+      <c r="D43" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="E44" s="24" t="s">
+      <c r="E43" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F44" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A46" s="67" t="s">
+      <c r="F43" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="35" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="21">
+      <c r="A45" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="66"/>
-      <c r="C46" s="66"/>
-      <c r="D46" s="66"/>
-      <c r="E46" s="66"/>
-      <c r="F46" s="66"/>
-      <c r="G46" s="66"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="65"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="65"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A35:A44"/>
-    <mergeCell ref="B35:B44"/>
+  <mergeCells count="14">
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="B34:B43"/>
+    <mergeCell ref="A23:A33"/>
+    <mergeCell ref="B23:B33"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B28:B34"/>
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="B1:G1"/>
@@ -2582,20 +2519,17 @@
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="A6:A13"/>
   </mergeCells>
-  <conditionalFormatting sqref="E30:G30 C32:C34 E32:G34 C31:G31 C6:G26 C35:G44 C28:G29">
+  <conditionalFormatting sqref="E29:G29 C31:C33 E31:G33 C30:G30 C6:G28 C34:G43">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:D30">
+  <conditionalFormatting sqref="C29:D29">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="36" orientation="portrait" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="26" max="16383" man="1"/>
-  </rowBreaks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Considerações da professora Rita
Alterações conforme considerações da Professora Rita
</commit_message>
<xml_diff>
--- a/Arquivos Excel/Safe & Sound.xlsx
+++ b/Arquivos Excel/Safe & Sound.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gih_m\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\GitHub\-ATV1-DMSQL\Arquivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C531264-672B-4AED-BC2F-8B38C0727A2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A353D2AE-3613-4B51-B0B8-0D1E48E1793D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projeto Safe&amp;Sound" sheetId="2" r:id="rId1"/>
@@ -523,7 +523,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1189,24 +1189,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1215,18 +1227,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1627,36 +1627,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39F60B7E-595C-4DED-A8B7-7A6F54C6BC44}">
   <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:B43"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.21875" customWidth="1"/>
-    <col min="2" max="2" width="54.21875" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1"/>
-    <col min="4" max="4" width="48.44140625" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.77734375" customWidth="1"/>
-    <col min="7" max="7" width="30.21875" customWidth="1"/>
-    <col min="8" max="15" width="8.5546875" customWidth="1"/>
-    <col min="16" max="17" width="7.77734375" customWidth="1"/>
-    <col min="18" max="1023" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="44.1796875" customWidth="1"/>
+    <col min="2" max="2" width="54.1796875" customWidth="1"/>
+    <col min="3" max="3" width="30.36328125" customWidth="1"/>
+    <col min="4" max="4" width="48.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.81640625" customWidth="1"/>
+    <col min="7" max="7" width="30.1796875" customWidth="1"/>
+    <col min="8" max="15" width="8.54296875" customWidth="1"/>
+    <col min="16" max="17" width="7.81640625" customWidth="1"/>
+    <col min="18" max="1023" width="8.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="20.399999999999999" customHeight="1">
+    <row r="1" spans="1:18" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1669,18 +1669,18 @@
       <c r="Q1" s="1"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18" ht="46.95" customHeight="1">
+    <row r="2" spans="1:18" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -1692,18 +1692,18 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="4"/>
     </row>
-    <row r="3" spans="1:18" s="6" customFormat="1" ht="81.75" customHeight="1" thickBot="1">
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="66" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -1715,7 +1715,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="15" thickBot="1">
+    <row r="4" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="10"/>
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
@@ -1726,7 +1726,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:18" ht="83.4" thickBot="1">
+    <row r="5" spans="1:18" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
         <v>47</v>
       </c>
@@ -1749,11 +1749,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="49.5" customHeight="1">
-      <c r="A6" s="54" t="s">
+    <row r="6" spans="1:18" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="63" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -1772,9 +1772,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="69">
-      <c r="A7" s="55"/>
-      <c r="B7" s="58"/>
+    <row r="7" spans="1:18" ht="70" x14ac:dyDescent="0.35">
+      <c r="A7" s="58"/>
+      <c r="B7" s="60"/>
       <c r="C7" s="21" t="s">
         <v>16</v>
       </c>
@@ -1791,9 +1791,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="96.6">
-      <c r="A8" s="55"/>
-      <c r="B8" s="58"/>
+    <row r="8" spans="1:18" ht="98" x14ac:dyDescent="0.35">
+      <c r="A8" s="58"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="22" t="s">
         <v>19</v>
       </c>
@@ -1810,9 +1810,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="150" customHeight="1">
-      <c r="A9" s="55"/>
-      <c r="B9" s="58"/>
+    <row r="9" spans="1:18" ht="150" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="58"/>
+      <c r="B9" s="60"/>
       <c r="C9" s="21" t="s">
         <v>18</v>
       </c>
@@ -1829,9 +1829,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="120.75" customHeight="1">
-      <c r="A10" s="55"/>
-      <c r="B10" s="58"/>
+    <row r="10" spans="1:18" ht="120.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="58"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="46" t="s">
         <v>59</v>
       </c>
@@ -1848,9 +1848,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="66.75" customHeight="1">
-      <c r="A11" s="55"/>
-      <c r="B11" s="58"/>
+    <row r="11" spans="1:18" ht="66.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="58"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="21" t="s">
         <v>21</v>
       </c>
@@ -1867,9 +1867,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="90" customHeight="1">
-      <c r="A12" s="55"/>
-      <c r="B12" s="58"/>
+    <row r="12" spans="1:18" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="58"/>
+      <c r="B12" s="60"/>
       <c r="C12" s="21" t="s">
         <v>22</v>
       </c>
@@ -1886,9 +1886,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="79.5" customHeight="1" thickBot="1">
-      <c r="A13" s="56"/>
-      <c r="B13" s="59"/>
+    <row r="13" spans="1:18" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="59"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="21" t="s">
         <v>25</v>
       </c>
@@ -1905,11 +1905,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="124.2">
-      <c r="A14" s="54" t="s">
+    <row r="14" spans="1:18" ht="126" x14ac:dyDescent="0.35">
+      <c r="A14" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="63" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="44" t="s">
@@ -1928,9 +1928,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="27.6">
-      <c r="A15" s="55"/>
-      <c r="B15" s="58"/>
+    <row r="15" spans="1:18" ht="28" x14ac:dyDescent="0.35">
+      <c r="A15" s="58"/>
+      <c r="B15" s="60"/>
       <c r="C15" s="29" t="s">
         <v>28</v>
       </c>
@@ -1947,9 +1947,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="55.2">
-      <c r="A16" s="55"/>
-      <c r="B16" s="58"/>
+    <row r="16" spans="1:18" ht="56" x14ac:dyDescent="0.35">
+      <c r="A16" s="58"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="29" t="s">
         <v>29</v>
       </c>
@@ -1966,9 +1966,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="97.2" thickBot="1">
-      <c r="A17" s="56"/>
-      <c r="B17" s="59"/>
+    <row r="17" spans="1:7" ht="98.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="59"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="47" t="s">
         <v>55</v>
       </c>
@@ -1985,11 +1985,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="69">
-      <c r="A18" s="54" t="s">
+    <row r="18" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+      <c r="A18" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="63" t="s">
         <v>30</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -2008,9 +2008,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="27.6">
-      <c r="A19" s="55"/>
-      <c r="B19" s="58"/>
+    <row r="19" spans="1:7" ht="28" x14ac:dyDescent="0.35">
+      <c r="A19" s="58"/>
+      <c r="B19" s="60"/>
       <c r="C19" s="29" t="s">
         <v>45</v>
       </c>
@@ -2027,9 +2027,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="41.4">
-      <c r="A20" s="55"/>
-      <c r="B20" s="58"/>
+    <row r="20" spans="1:7" ht="42" x14ac:dyDescent="0.35">
+      <c r="A20" s="58"/>
+      <c r="B20" s="60"/>
       <c r="C20" s="33" t="s">
         <v>31</v>
       </c>
@@ -2046,9 +2046,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="96.6">
-      <c r="A21" s="55"/>
-      <c r="B21" s="58"/>
+    <row r="21" spans="1:7" ht="98" x14ac:dyDescent="0.35">
+      <c r="A21" s="58"/>
+      <c r="B21" s="60"/>
       <c r="C21" s="29" t="s">
         <v>33</v>
       </c>
@@ -2065,9 +2065,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="97.2" thickBot="1">
-      <c r="A22" s="56"/>
-      <c r="B22" s="59"/>
+    <row r="22" spans="1:7" ht="98.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="59"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="47" t="s">
         <v>55</v>
       </c>
@@ -2084,11 +2084,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" customHeight="1">
-      <c r="A23" s="55" t="s">
+    <row r="23" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="60" t="s">
         <v>34</v>
       </c>
       <c r="C23" s="31" t="s">
@@ -2107,9 +2107,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="55.2">
-      <c r="A24" s="55"/>
-      <c r="B24" s="58"/>
+    <row r="24" spans="1:7" ht="56" x14ac:dyDescent="0.35">
+      <c r="A24" s="58"/>
+      <c r="B24" s="60"/>
       <c r="C24" s="29" t="s">
         <v>36</v>
       </c>
@@ -2126,9 +2126,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="96.6">
-      <c r="A25" s="55"/>
-      <c r="B25" s="58"/>
+    <row r="25" spans="1:7" ht="98" x14ac:dyDescent="0.35">
+      <c r="A25" s="58"/>
+      <c r="B25" s="60"/>
       <c r="C25" s="22" t="s">
         <v>19</v>
       </c>
@@ -2145,9 +2145,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="110.4">
-      <c r="A26" s="55"/>
-      <c r="B26" s="58"/>
+    <row r="26" spans="1:7" ht="112" x14ac:dyDescent="0.35">
+      <c r="A26" s="58"/>
+      <c r="B26" s="60"/>
       <c r="C26" s="21" t="s">
         <v>58</v>
       </c>
@@ -2164,9 +2164,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="138">
-      <c r="A27" s="55"/>
-      <c r="B27" s="58"/>
+    <row r="27" spans="1:7" ht="140" x14ac:dyDescent="0.35">
+      <c r="A27" s="58"/>
+      <c r="B27" s="60"/>
       <c r="C27" s="21" t="s">
         <v>18</v>
       </c>
@@ -2183,9 +2183,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="69">
-      <c r="A28" s="55"/>
-      <c r="B28" s="58"/>
+    <row r="28" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+      <c r="A28" s="58"/>
+      <c r="B28" s="60"/>
       <c r="C28" s="50" t="s">
         <v>16</v>
       </c>
@@ -2202,9 +2202,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="124.2">
-      <c r="A29" s="55"/>
-      <c r="B29" s="58"/>
+    <row r="29" spans="1:7" ht="126" x14ac:dyDescent="0.35">
+      <c r="A29" s="58"/>
+      <c r="B29" s="60"/>
       <c r="C29" s="52" t="s">
         <v>67</v>
       </c>
@@ -2221,9 +2221,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="27.6">
-      <c r="A30" s="55"/>
-      <c r="B30" s="58"/>
+    <row r="30" spans="1:7" ht="28" x14ac:dyDescent="0.35">
+      <c r="A30" s="58"/>
+      <c r="B30" s="60"/>
       <c r="C30" s="29" t="s">
         <v>28</v>
       </c>
@@ -2240,9 +2240,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="69">
-      <c r="A31" s="55"/>
-      <c r="B31" s="58"/>
+    <row r="31" spans="1:7" ht="70" x14ac:dyDescent="0.35">
+      <c r="A31" s="58"/>
+      <c r="B31" s="60"/>
       <c r="C31" s="29" t="s">
         <v>37</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>68</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F31" s="32" t="s">
         <v>14</v>
@@ -2259,9 +2259,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="55.2">
-      <c r="A32" s="55"/>
-      <c r="B32" s="58"/>
+    <row r="32" spans="1:7" ht="56" x14ac:dyDescent="0.35">
+      <c r="A32" s="58"/>
+      <c r="B32" s="60"/>
       <c r="C32" s="29" t="s">
         <v>38</v>
       </c>
@@ -2269,18 +2269,18 @@
         <v>39</v>
       </c>
       <c r="E32" s="32" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F32" s="32" t="s">
         <v>14</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="97.2" thickBot="1">
-      <c r="A33" s="56"/>
-      <c r="B33" s="59"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="98.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="59"/>
+      <c r="B33" s="61"/>
       <c r="C33" s="24" t="s">
         <v>40</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>69</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>17</v>
@@ -2297,11 +2297,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="41.1" customHeight="1" thickBot="1">
-      <c r="A34" s="63" t="s">
+    <row r="34" spans="1:7" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="57" t="s">
         <v>70</v>
       </c>
       <c r="C34" s="26" t="s">
@@ -2320,9 +2320,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="55.8" thickBot="1">
-      <c r="A35" s="63"/>
-      <c r="B35" s="64"/>
+    <row r="35" spans="1:7" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A35" s="56"/>
+      <c r="B35" s="57"/>
       <c r="C35" s="29" t="s">
         <v>72</v>
       </c>
@@ -2339,9 +2339,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="42" thickBot="1">
-      <c r="A36" s="63"/>
-      <c r="B36" s="64"/>
+    <row r="36" spans="1:7" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="56"/>
+      <c r="B36" s="57"/>
       <c r="C36" s="29" t="s">
         <v>43</v>
       </c>
@@ -2358,9 +2358,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="69.599999999999994" thickBot="1">
-      <c r="A37" s="63"/>
-      <c r="B37" s="64"/>
+    <row r="37" spans="1:7" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="56"/>
+      <c r="B37" s="57"/>
       <c r="C37" s="29" t="s">
         <v>19</v>
       </c>
@@ -2377,9 +2377,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="111" thickBot="1">
-      <c r="A38" s="63"/>
-      <c r="B38" s="64"/>
+    <row r="38" spans="1:7" ht="112.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A38" s="56"/>
+      <c r="B38" s="57"/>
       <c r="C38" s="21" t="s">
         <v>58</v>
       </c>
@@ -2396,9 +2396,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="58.95" customHeight="1" thickBot="1">
-      <c r="A39" s="63"/>
-      <c r="B39" s="64"/>
+    <row r="39" spans="1:7" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A39" s="56"/>
+      <c r="B39" s="57"/>
       <c r="C39" s="29" t="s">
         <v>18</v>
       </c>
@@ -2415,9 +2415,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="69.599999999999994" thickBot="1">
-      <c r="A40" s="63"/>
-      <c r="B40" s="64"/>
+    <row r="40" spans="1:7" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A40" s="56"/>
+      <c r="B40" s="57"/>
       <c r="C40" s="21" t="s">
         <v>16</v>
       </c>
@@ -2434,9 +2434,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="42" thickBot="1">
-      <c r="A41" s="63"/>
-      <c r="B41" s="64"/>
+    <row r="41" spans="1:7" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="56"/>
+      <c r="B41" s="57"/>
       <c r="C41" s="29" t="s">
         <v>31</v>
       </c>
@@ -2453,9 +2453,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="40.200000000000003" customHeight="1" thickBot="1">
-      <c r="A42" s="63"/>
-      <c r="B42" s="64"/>
+    <row r="42" spans="1:7" ht="40.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="56"/>
+      <c r="B42" s="57"/>
       <c r="C42" s="29" t="s">
         <v>45</v>
       </c>
@@ -2472,9 +2472,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="69.599999999999994" thickBot="1">
-      <c r="A43" s="63"/>
-      <c r="B43" s="64"/>
+    <row r="43" spans="1:7" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="56"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="24" t="s">
         <v>38</v>
       </c>
@@ -2491,24 +2491,19 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="21">
-      <c r="A45" s="66" t="s">
+    <row r="45" spans="1:7" ht="21" x14ac:dyDescent="0.5">
+      <c r="A45" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="B45" s="65"/>
-      <c r="C45" s="65"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="B34:B43"/>
-    <mergeCell ref="A23:A33"/>
-    <mergeCell ref="B23:B33"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B18:B22"/>
     <mergeCell ref="A14:A17"/>
@@ -2518,6 +2513,11 @@
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="A6:A13"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="B34:B43"/>
+    <mergeCell ref="A23:A33"/>
+    <mergeCell ref="B23:B33"/>
   </mergeCells>
   <conditionalFormatting sqref="E29:G29 C31:C33 E31:G33 C30:G30 C6:G28 C34:G43">
     <cfRule type="expression" dxfId="1" priority="2">

</xml_diff>